<commit_message>
Second order groups configurations for Environmental properties done!
</commit_message>
<xml_diff>
--- a/data/HukkerikarEnvironmental.xlsx
+++ b/data/HukkerikarEnvironmental.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115" activeTab="3" xr2:uid="{B1B8E9E2-0821-49EE-A8A7-D989EA31A508}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115" tabRatio="724" activeTab="1" xr2:uid="{B1B8E9E2-0821-49EE-A8A7-D989EA31A508}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8790" activeTab="1" xr2:uid="{9DF4B5E0-0503-411D-9815-9AD522F5F236}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstOrder" sheetId="2" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="690">
   <si>
     <t>Group</t>
   </si>
@@ -1903,9 +1904,6 @@
     <t>ACRY</t>
   </si>
   <si>
-    <t>CL-(C=C)</t>
-  </si>
-  <si>
     <t>CLCC</t>
   </si>
   <si>
@@ -2078,13 +2076,326 @@
   </si>
   <si>
     <t>Equivalence</t>
+  </si>
+  <si>
+    <t>Configurations</t>
+  </si>
+  <si>
+    <t>3(1).1</t>
+  </si>
+  <si>
+    <t>4(1)(1).1</t>
+  </si>
+  <si>
+    <t>3(1).3.1</t>
+  </si>
+  <si>
+    <t>4(1)(1).3.1</t>
+  </si>
+  <si>
+    <t>4(1)(1).4(1)(1)</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.70|8|7|6|5</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.1</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.2</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.3|4</t>
+  </si>
+  <si>
+    <t>20.3|4</t>
+  </si>
+  <si>
+    <t>18.2/19.1</t>
+  </si>
+  <si>
+    <t>18.3|4</t>
+  </si>
+  <si>
+    <t>42.3|4</t>
+  </si>
+  <si>
+    <t>21.3|4</t>
+  </si>
+  <si>
+    <t>77.19|18/77.2|3|4.18|19/22.18|19</t>
+  </si>
+  <si>
+    <t>2|3|4(82|81|14).29|30|85|32|33|35</t>
+  </si>
+  <si>
+    <t>29|30|85.29|30|85</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.1</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.2</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.3|4</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>(CH3)2C</t>
+  </si>
+  <si>
+    <t>CHn=CHm-CHp=CHk</t>
+  </si>
+  <si>
+    <t>CH3-CHm=CHn</t>
+  </si>
+  <si>
+    <t>CH2--CHm=CHn</t>
+  </si>
+  <si>
+    <t>CH-CHm=CHn/CCHm=CHn</t>
+  </si>
+  <si>
+    <t>CHCHO/CCHO</t>
+  </si>
+  <si>
+    <t>CH3COCH/CH3COC</t>
+  </si>
+  <si>
+    <t>CHCOOH/CCOOH</t>
+  </si>
+  <si>
+    <t>CH3COOCH/CH3COOC</t>
+  </si>
+  <si>
+    <t>CHm(OH)CHn(OH)</t>
+  </si>
+  <si>
+    <t>CHm(OH)CHn(NHp)</t>
+  </si>
+  <si>
+    <t>CHm(NH2)CHn(NH2)</t>
+  </si>
+  <si>
+    <t>CHm-O-CHn=CHp</t>
+  </si>
+  <si>
+    <t>CHm=CHnBr</t>
+  </si>
+  <si>
+    <t>CHm=CHnI</t>
+  </si>
+  <si>
+    <t>CHm(NH2)COOH</t>
+  </si>
+  <si>
+    <t>38.3|4</t>
+  </si>
+  <si>
+    <t>33.2/34.1</t>
+  </si>
+  <si>
+    <t>33.3|4</t>
+  </si>
+  <si>
+    <t>31.3|4</t>
+  </si>
+  <si>
+    <t>40.3|4</t>
+  </si>
+  <si>
+    <t>29.69|70</t>
+  </si>
+  <si>
+    <t>34(1).29/18.2|3|4.29</t>
+  </si>
+  <si>
+    <r>
+      <t>22.14/77.2.14/77.3.81</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/77</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.4.82</t>
+    </r>
+  </si>
+  <si>
+    <t>2|3|4(14|81|82).2|3|4(14|81|82)</t>
+  </si>
+  <si>
+    <t>19(1).14/18.2|3|4.14|81|82</t>
+  </si>
+  <si>
+    <t>2|3|4(29).2|3|4(29)</t>
+  </si>
+  <si>
+    <t>54|55|56.54|55|56</t>
+  </si>
+  <si>
+    <t>32|33.29|30|85</t>
+  </si>
+  <si>
+    <t>58|59.54|55|56</t>
+  </si>
+  <si>
+    <t>91.2|3.2|3.91</t>
+  </si>
+  <si>
+    <t>86.2|3.2|3.86</t>
+  </si>
+  <si>
+    <t>2|3|4(29).54|55|56|58|59|61</t>
+  </si>
+  <si>
+    <t>29|30|85|32|33|35.42</t>
+  </si>
+  <si>
+    <t>54|55|56|58|59|61.31</t>
+  </si>
+  <si>
+    <t>31.2|3.31</t>
+  </si>
+  <si>
+    <t>42.2|3.42</t>
+  </si>
+  <si>
+    <t>42.2|3.2|3.42</t>
+  </si>
+  <si>
+    <t>31.2|3.2|3.31</t>
+  </si>
+  <si>
+    <t>29.2|3.31</t>
+  </si>
+  <si>
+    <t>14|81|82.2|3.42</t>
+  </si>
+  <si>
+    <t>54|55.2|3.31</t>
+  </si>
+  <si>
+    <t>29|30.2|3.42</t>
+  </si>
+  <si>
+    <t>24.2|3.42</t>
+  </si>
+  <si>
+    <t>49.2|3.31</t>
+  </si>
+  <si>
+    <t>60.2|3.42</t>
+  </si>
+  <si>
+    <t>68|69.68|69</t>
+  </si>
+  <si>
+    <t>29.2|3.68|69</t>
+  </si>
+  <si>
+    <t>14|81|82.2|3.41</t>
+  </si>
+  <si>
+    <t>138|139.2|3.31</t>
+  </si>
+  <si>
+    <t>77.2|3.2|3.77</t>
+  </si>
+  <si>
+    <t>48.2|3.2|3.48</t>
+  </si>
+  <si>
+    <t>41|42.41|42</t>
+  </si>
+  <si>
+    <t>68|69.48</t>
+  </si>
+  <si>
+    <t>24|25|26.5|6|7|8|70</t>
+  </si>
+  <si>
+    <t>49|50|51.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>129.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>Brexceptasabove</t>
+  </si>
+  <si>
+    <t>Iexceptasabove</t>
+  </si>
+  <si>
+    <t>Clexceptasabove</t>
+  </si>
+  <si>
+    <t>Cl-(C=C)</t>
+  </si>
+  <si>
+    <t>64.5|6|7|8|70</t>
+  </si>
+  <si>
+    <t>128.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>127.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>63.5|6|7|8|70</t>
+  </si>
+  <si>
+    <t>130.9|8|7|6|5</t>
+  </si>
+  <si>
+    <t>COCH2COO/COCHCOO/COCCOO</t>
+  </si>
+  <si>
+    <t>48.34|35/48.2|3.33|34|35/41|42.33|34|35</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.77.1|2|3|4</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.48.1|2|3|4</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.20</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.38</t>
+  </si>
+  <si>
+    <t>70|8|7|6|5.42</t>
+  </si>
+  <si>
+    <t>9|8|7|6|5.31</t>
+  </si>
+  <si>
+    <t>UNIFAC Configurations</t>
+  </si>
+  <si>
+    <t>Gani-Const Groups</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2142,6 +2453,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2364,7 +2686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2461,6 +2783,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2497,90 +2825,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2687,6 +2931,43 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2804,6 +3085,53 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2818,22 +3146,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2705E1D5-5341-4401-BFD2-EC8497DDB141}" name="Table2" displayName="Table2" ref="A1:D129" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2705E1D5-5341-4401-BFD2-EC8497DDB141}" name="Table2" displayName="Table2" ref="A1:D129" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97ACAD8E-9361-4D28-8EB8-A9AAF9F8DCA2}" name="Column1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{26DFE1A7-791C-482C-BA42-0807897D8853}" name="UNIFAC" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{3BA6543D-AB2D-4401-94D1-B819865C8B13}" name="Column2" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{5029B48F-C04B-4C3B-B41A-540C53A98D41}" name="Column3" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{97ACAD8E-9361-4D28-8EB8-A9AAF9F8DCA2}" name="Column1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{26DFE1A7-791C-482C-BA42-0807897D8853}" name="UNIFAC" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{3BA6543D-AB2D-4401-94D1-B819865C8B13}" name="Column2" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5029B48F-C04B-4C3B-B41A-540C53A98D41}" name="Column3" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A2791E3-94F0-467E-B931-F72DC38CF0D4}" name="Table3" displayName="Table3" ref="F1:H256" totalsRowShown="0" headerRowDxfId="1" dataDxfId="11" headerRowBorderDxfId="2" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A2791E3-94F0-467E-B931-F72DC38CF0D4}" name="Table3" displayName="Table3" ref="F1:H257" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{664DC018-5679-4754-BCB8-F3FC7827B4AA}" name="Column1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{EDE3EE0B-9708-4CFB-B04C-488B8771C767}" name="HUKKERIKAR" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{664DC018-5679-4754-BCB8-F3FC7827B4AA}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{EDE3EE0B-9708-4CFB-B04C-488B8771C767}" name="HUKKERIKAR" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{667EC796-0E48-4D46-BCB5-080434B1EEC5}" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3139,8 +3467,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CF915C-548F-44E5-A457-8BD61E3FF56A}">
   <dimension ref="A1:X221"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H176" sqref="H176"/>
+    <sheetView topLeftCell="I74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L190" sqref="L190"/>
+    </sheetView>
+    <sheetView topLeftCell="A22" workbookViewId="1">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10320,7 +10651,7 @@
       <c r="A128" s="1">
         <v>127</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="38" t="s">
         <v>127</v>
       </c>
       <c r="C128" s="2">
@@ -15090,18 +15421,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F60655-82C2-4DD7-8FC9-7DBEF022EFA3}">
-  <dimension ref="A1:U131"/>
+  <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -15163,8 +15498,17 @@
       <c r="U1" s="6" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V1" s="39" t="s">
+        <v>592</v>
+      </c>
+      <c r="W1" s="39" t="s">
+        <v>688</v>
+      </c>
+      <c r="X1" s="39" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -15228,8 +15572,17 @@
       <c r="U2" s="2">
         <v>0.15140000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V2" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -15293,8 +15646,17 @@
       <c r="U3" s="2">
         <v>-0.19620000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -15332,8 +15694,17 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -15369,8 +15740,17 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V5" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -15404,8 +15784,17 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -15469,8 +15858,17 @@
       <c r="U7" s="2">
         <v>-0.2213</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V7" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -15534,8 +15932,17 @@
       <c r="U8" s="2">
         <v>-2.9600000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -15599,8 +16006,17 @@
       <c r="U9" s="2">
         <v>0.2059</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -15662,8 +16078,17 @@
       <c r="U10" s="2">
         <v>-0.50260000000000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -15697,8 +16122,17 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V11" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -15760,8 +16194,17 @@
       <c r="U12" s="2">
         <v>-0.14879999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -15799,8 +16242,17 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V13" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -15862,8 +16314,17 @@
       <c r="U14" s="2">
         <v>-0.16309999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -15911,8 +16372,17 @@
         <v>-9.06E-2</v>
       </c>
       <c r="U15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V15" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -15946,8 +16416,13 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -16011,8 +16486,17 @@
       <c r="U17" s="2">
         <v>-0.17460000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V17" s="2">
+        <v>29.3</v>
+      </c>
+      <c r="W17" s="2">
+        <v>81.3</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -16074,8 +16558,17 @@
       <c r="U18" s="2">
         <v>-0.1091</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V18" s="2">
+        <v>29.4</v>
+      </c>
+      <c r="W18" s="2">
+        <v>82.4</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -16107,8 +16600,15 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V19" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -16140,8 +16640,13 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V20" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -16201,8 +16706,13 @@
       <c r="U21" s="2">
         <v>0.18509999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V21" s="2"/>
+      <c r="W21" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -16256,8 +16766,17 @@
         <v>-0.25509999999999999</v>
       </c>
       <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V22" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -16309,8 +16828,17 @@
         <v>-1.0750999999999999</v>
       </c>
       <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -16346,8 +16874,17 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V24" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -16381,8 +16918,15 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -16410,8 +16954,15 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V26" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -16467,8 +17018,17 @@
       <c r="U27" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V27" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -16498,8 +17058,15 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V28" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -16533,8 +17100,15 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V29" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="X29" s="2"/>
+    </row>
+    <row r="30" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -16568,8 +17142,15 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V30" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="X30" s="2"/>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -16597,8 +17178,15 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V31" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="X31" s="2"/>
+    </row>
+    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -16626,8 +17214,15 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V32" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="X32" s="2"/>
+    </row>
+    <row r="33" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -16661,8 +17256,13 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V33" s="2">
+        <v>139.32</v>
+      </c>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+    </row>
+    <row r="34" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -16692,8 +17292,15 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V34" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="X34" s="2"/>
+    </row>
+    <row r="35" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -16725,8 +17332,15 @@
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V35" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="W35" s="2">
+        <v>41.41</v>
+      </c>
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -16756,8 +17370,15 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V36" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="X36" s="2"/>
+    </row>
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -16785,8 +17406,15 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V37" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="W37" s="2">
+        <v>60.64</v>
+      </c>
+      <c r="X37" s="2"/>
+    </row>
+    <row r="38" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -16830,8 +17458,15 @@
         <v>0.4819</v>
       </c>
       <c r="U38" s="2"/>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V38" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="X38" s="2"/>
+    </row>
+    <row r="39" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -16895,8 +17530,15 @@
       <c r="U39" s="2">
         <v>1.3833</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V39" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="W39" s="2">
+        <v>22.22</v>
+      </c>
+      <c r="X39" s="2"/>
+    </row>
+    <row r="40" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -16926,8 +17568,15 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V40" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="W40" s="2">
+        <v>41.77</v>
+      </c>
+      <c r="X40" s="2"/>
+    </row>
+    <row r="41" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -16969,8 +17618,17 @@
         <v>-1.0732999999999999</v>
       </c>
       <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V41" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -17002,8 +17660,17 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V42" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -17047,8 +17714,13 @@
         <v>-2.8199999999999999E-2</v>
       </c>
       <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V43" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -17094,8 +17766,17 @@
       <c r="U44" s="2">
         <v>-6.7199999999999996E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V44" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -17123,8 +17804,17 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V45" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -17188,8 +17878,15 @@
       <c r="U46" s="2">
         <v>-6.7000000000000002E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V46" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="W46" s="2">
+        <v>69</v>
+      </c>
+      <c r="X46" s="2"/>
+    </row>
+    <row r="47" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -17251,8 +17948,11 @@
       <c r="U47" s="2">
         <v>-0.9052</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+    </row>
+    <row r="48" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -17314,8 +18014,15 @@
       <c r="U48" s="2">
         <v>7.9500000000000001E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V48" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="X48" s="2"/>
+    </row>
+    <row r="49" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -17377,8 +18084,15 @@
       <c r="U49" s="2">
         <v>-1.1983999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V49" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="X49" s="2"/>
+    </row>
+    <row r="50" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -17426,8 +18140,15 @@
         <v>-0.83789999999999998</v>
       </c>
       <c r="U50" s="2"/>
-    </row>
-    <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V50" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="X50" s="2"/>
+    </row>
+    <row r="51" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -17475,8 +18196,11 @@
         <v>-0.52939999999999998</v>
       </c>
       <c r="U51" s="2"/>
-    </row>
-    <row r="52" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+    </row>
+    <row r="52" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -17522,8 +18246,11 @@
         <v>0.50229999999999997</v>
       </c>
       <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2"/>
+    </row>
+    <row r="53" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -17583,8 +18310,11 @@
       <c r="U53" s="2">
         <v>0.14940000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2"/>
+    </row>
+    <row r="54" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -17644,8 +18374,11 @@
       <c r="U54" s="2">
         <v>-0.1477</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V54" s="2"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+    </row>
+    <row r="55" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -17693,8 +18426,11 @@
       <c r="U55" s="2">
         <v>5.2600000000000001E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+    </row>
+    <row r="56" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -17724,8 +18460,11 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-    </row>
-    <row r="57" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+    </row>
+    <row r="57" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -17753,8 +18492,11 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
-    </row>
-    <row r="58" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+    </row>
+    <row r="58" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -17786,8 +18528,11 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-    </row>
-    <row r="59" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
+      <c r="X58" s="2"/>
+    </row>
+    <row r="59" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -17833,8 +18578,11 @@
       <c r="U59" s="2">
         <v>4.9299999999999997E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2"/>
+    </row>
+    <row r="60" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -17878,8 +18626,11 @@
       <c r="U60" s="2">
         <v>0.33960000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V60" s="2"/>
+      <c r="W60" s="2"/>
+      <c r="X60" s="2"/>
+    </row>
+    <row r="61" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -17907,8 +18658,11 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-    </row>
-    <row r="62" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V61" s="2"/>
+      <c r="W61" s="2"/>
+      <c r="X61" s="2"/>
+    </row>
+    <row r="62" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -17934,8 +18688,11 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-    </row>
-    <row r="63" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V62" s="2"/>
+      <c r="W62" s="2"/>
+      <c r="X62" s="2"/>
+    </row>
+    <row r="63" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -17965,8 +18722,11 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-    </row>
-    <row r="64" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V63" s="2"/>
+      <c r="W63" s="2"/>
+      <c r="X63" s="2"/>
+    </row>
+    <row r="64" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -18028,8 +18788,11 @@
       <c r="U64" s="2">
         <v>-6.7900000000000002E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V64" s="2"/>
+      <c r="W64" s="2"/>
+      <c r="X64" s="2"/>
+    </row>
+    <row r="65" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -18089,8 +18852,11 @@
       <c r="U65" s="2">
         <v>-0.44290000000000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V65" s="2"/>
+      <c r="W65" s="2"/>
+      <c r="X65" s="2"/>
+    </row>
+    <row r="66" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -18124,8 +18890,11 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
-    </row>
-    <row r="67" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V66" s="2"/>
+      <c r="W66" s="2"/>
+      <c r="X66" s="2"/>
+    </row>
+    <row r="67" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -18189,8 +18958,11 @@
       <c r="U67" s="2">
         <v>-8.0799999999999997E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V67" s="2"/>
+      <c r="W67" s="2"/>
+      <c r="X67" s="2"/>
+    </row>
+    <row r="68" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -18252,8 +19024,11 @@
       <c r="U68" s="2">
         <v>-0.27910000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+    </row>
+    <row r="69" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -18315,8 +19090,11 @@
       <c r="U69" s="2">
         <v>-7.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+      <c r="X69" s="2"/>
+    </row>
+    <row r="70" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -18372,8 +19150,11 @@
       <c r="U70" s="2">
         <v>-2.0500000000000001E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V70" s="2"/>
+      <c r="W70" s="2"/>
+      <c r="X70" s="2"/>
+    </row>
+    <row r="71" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -18417,8 +19198,11 @@
       <c r="U71" s="2">
         <v>-0.44640000000000002</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V71" s="2"/>
+      <c r="W71" s="2"/>
+      <c r="X71" s="2"/>
+    </row>
+    <row r="72" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -18462,8 +19246,11 @@
       <c r="U72" s="2">
         <v>0.4229</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V72" s="2"/>
+      <c r="W72" s="2"/>
+      <c r="X72" s="2"/>
+    </row>
+    <row r="73" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -18527,8 +19314,11 @@
       <c r="U73" s="2">
         <v>0.23910000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V73" s="2"/>
+      <c r="W73" s="2"/>
+      <c r="X73" s="2"/>
+    </row>
+    <row r="74" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -18588,8 +19378,11 @@
       <c r="U74" s="2">
         <v>-0.34089999999999998</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V74" s="2"/>
+      <c r="W74" s="2"/>
+      <c r="X74" s="2"/>
+    </row>
+    <row r="75" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -18633,8 +19426,11 @@
       <c r="U75" s="2">
         <v>0.224</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V75" s="2"/>
+      <c r="W75" s="2"/>
+      <c r="X75" s="2"/>
+    </row>
+    <row r="76" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -18696,8 +19492,11 @@
       <c r="U76" s="2">
         <v>5.9400000000000001E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V76" s="2"/>
+      <c r="W76" s="2"/>
+      <c r="X76" s="2"/>
+    </row>
+    <row r="77" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -18761,8 +19560,11 @@
       <c r="U77" s="2">
         <v>-0.18679999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V77" s="2"/>
+      <c r="W77" s="2"/>
+      <c r="X77" s="2"/>
+    </row>
+    <row r="78" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -18826,8 +19628,11 @@
       <c r="U78" s="2">
         <v>0.25569999999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V78" s="2"/>
+      <c r="W78" s="2"/>
+      <c r="X78" s="2"/>
+    </row>
+    <row r="79" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -18877,8 +19682,11 @@
       <c r="U79" s="2">
         <v>2.53E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V79" s="2"/>
+      <c r="W79" s="2"/>
+      <c r="X79" s="2"/>
+    </row>
+    <row r="80" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -18914,8 +19722,11 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
-    </row>
-    <row r="81" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V80" s="2"/>
+      <c r="W80" s="2"/>
+      <c r="X80" s="2"/>
+    </row>
+    <row r="81" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -18977,8 +19788,11 @@
       <c r="U81" s="2">
         <v>0.62880000000000003</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V81" s="2"/>
+      <c r="W81" s="2"/>
+      <c r="X81" s="2"/>
+    </row>
+    <row r="82" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -19036,8 +19850,11 @@
       <c r="U82" s="2">
         <v>0.4768</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V82" s="2"/>
+      <c r="W82" s="2"/>
+      <c r="X82" s="2"/>
+    </row>
+    <row r="83" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -19099,8 +19916,11 @@
       <c r="U83" s="2">
         <v>-0.13869999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V83" s="2"/>
+      <c r="W83" s="2"/>
+      <c r="X83" s="2"/>
+    </row>
+    <row r="84" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -19128,8 +19948,11 @@
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
       <c r="U84" s="2"/>
-    </row>
-    <row r="85" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V84" s="2"/>
+      <c r="W84" s="2"/>
+      <c r="X84" s="2"/>
+    </row>
+    <row r="85" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -19181,8 +20004,11 @@
         <v>0.49630000000000002</v>
       </c>
       <c r="U85" s="2"/>
-    </row>
-    <row r="86" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V85" s="2"/>
+      <c r="W85" s="2"/>
+      <c r="X85" s="2"/>
+    </row>
+    <row r="86" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -19226,8 +20052,11 @@
       <c r="U86" s="2">
         <v>-0.43</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V86" s="2"/>
+      <c r="W86" s="2"/>
+      <c r="X86" s="2"/>
+    </row>
+    <row r="87" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -19275,8 +20104,11 @@
       <c r="U87" s="2">
         <v>-0.24249999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V87" s="2"/>
+      <c r="W87" s="2"/>
+      <c r="X87" s="2"/>
+    </row>
+    <row r="88" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -19322,8 +20154,11 @@
         <v>-1.0499000000000001</v>
       </c>
       <c r="U88" s="2"/>
-    </row>
-    <row r="89" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V88" s="2"/>
+      <c r="W88" s="2"/>
+      <c r="X88" s="2"/>
+    </row>
+    <row r="89" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -19353,8 +20188,11 @@
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
-    </row>
-    <row r="90" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V89" s="2"/>
+      <c r="W89" s="2"/>
+      <c r="X89" s="2"/>
+    </row>
+    <row r="90" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -19384,8 +20222,11 @@
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
       <c r="U90" s="2"/>
-    </row>
-    <row r="91" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V90" s="2"/>
+      <c r="W90" s="2"/>
+      <c r="X90" s="2"/>
+    </row>
+    <row r="91" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -19431,8 +20272,11 @@
         <v>0.68620000000000003</v>
       </c>
       <c r="U91" s="2"/>
-    </row>
-    <row r="92" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V91" s="2"/>
+      <c r="W91" s="2"/>
+      <c r="X91" s="2"/>
+    </row>
+    <row r="92" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -19474,8 +20318,11 @@
         <v>1.9332</v>
       </c>
       <c r="U92" s="2"/>
-    </row>
-    <row r="93" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V92" s="2"/>
+      <c r="W92" s="2"/>
+      <c r="X92" s="2"/>
+    </row>
+    <row r="93" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -19505,8 +20352,11 @@
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
       <c r="U93" s="2"/>
-    </row>
-    <row r="94" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V93" s="2"/>
+      <c r="W93" s="2"/>
+      <c r="X93" s="2"/>
+    </row>
+    <row r="94" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -19550,8 +20400,11 @@
       <c r="U94" s="2">
         <v>0.35410000000000003</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V94" s="2"/>
+      <c r="W94" s="2"/>
+      <c r="X94" s="2"/>
+    </row>
+    <row r="95" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -19585,8 +20438,11 @@
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
       <c r="U95" s="2"/>
-    </row>
-    <row r="96" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V95" s="2"/>
+      <c r="W95" s="2"/>
+      <c r="X95" s="2"/>
+    </row>
+    <row r="96" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -19642,8 +20498,11 @@
       <c r="U96" s="2">
         <v>5.7700000000000001E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V96" s="2"/>
+      <c r="W96" s="2"/>
+      <c r="X96" s="2"/>
+    </row>
+    <row r="97" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -19671,8 +20530,11 @@
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
       <c r="U97" s="2"/>
-    </row>
-    <row r="98" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V97" s="2"/>
+      <c r="W97" s="2"/>
+      <c r="X97" s="2"/>
+    </row>
+    <row r="98" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -19732,8 +20594,11 @@
       <c r="U98" s="2">
         <v>4.2599999999999999E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V98" s="2"/>
+      <c r="W98" s="2"/>
+      <c r="X98" s="2"/>
+    </row>
+    <row r="99" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -19779,8 +20644,11 @@
         <v>-0.67259999999999998</v>
       </c>
       <c r="U99" s="2"/>
-    </row>
-    <row r="100" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V99" s="2"/>
+      <c r="W99" s="2"/>
+      <c r="X99" s="2"/>
+    </row>
+    <row r="100" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -19844,8 +20712,11 @@
       <c r="U100" s="2">
         <v>-3.6799999999999999E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V100" s="2"/>
+      <c r="W100" s="2"/>
+      <c r="X100" s="2"/>
+    </row>
+    <row r="101" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -19909,8 +20780,11 @@
       <c r="U101" s="2">
         <v>-4.2700000000000002E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V101" s="2"/>
+      <c r="W101" s="2"/>
+      <c r="X101" s="2"/>
+    </row>
+    <row r="102" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -19960,8 +20834,11 @@
         <v>-0.50700000000000001</v>
       </c>
       <c r="U102" s="2"/>
-    </row>
-    <row r="103" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V102" s="2"/>
+      <c r="W102" s="2"/>
+      <c r="X102" s="2"/>
+    </row>
+    <row r="103" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -20023,8 +20900,11 @@
       <c r="U103" s="2">
         <v>0.15229999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V103" s="2"/>
+      <c r="W103" s="2"/>
+      <c r="X103" s="2"/>
+    </row>
+    <row r="104" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -20084,8 +20964,11 @@
       <c r="U104" s="2">
         <v>0.27100000000000002</v>
       </c>
-    </row>
-    <row r="105" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V104" s="2"/>
+      <c r="W104" s="2"/>
+      <c r="X104" s="2"/>
+    </row>
+    <row r="105" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -20149,8 +21032,11 @@
       <c r="U105" s="2">
         <v>0.17799999999999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V105" s="2"/>
+      <c r="W105" s="2"/>
+      <c r="X105" s="2"/>
+    </row>
+    <row r="106" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -20214,8 +21100,11 @@
       <c r="U106" s="2">
         <v>-0.12089999999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V106" s="2"/>
+      <c r="W106" s="2"/>
+      <c r="X106" s="2"/>
+    </row>
+    <row r="107" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -20279,8 +21168,11 @@
       <c r="U107" s="2">
         <v>0.16370000000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V107" s="2"/>
+      <c r="W107" s="2"/>
+      <c r="X107" s="2"/>
+    </row>
+    <row r="108" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -20344,8 +21236,11 @@
       <c r="U108" s="2">
         <v>-0.43969999999999998</v>
       </c>
-    </row>
-    <row r="109" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V108" s="2"/>
+      <c r="W108" s="2"/>
+      <c r="X108" s="2"/>
+    </row>
+    <row r="109" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -20409,8 +21304,11 @@
       <c r="U109" s="2">
         <v>-0.11650000000000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V109" s="2"/>
+      <c r="W109" s="2"/>
+      <c r="X109" s="2"/>
+    </row>
+    <row r="110" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -20474,8 +21372,11 @@
       <c r="U110" s="2">
         <v>-4.19E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V110" s="2"/>
+      <c r="W110" s="2"/>
+      <c r="X110" s="2"/>
+    </row>
+    <row r="111" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -20537,8 +21438,11 @@
       <c r="U111" s="2">
         <v>-9.0899999999999995E-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V111" s="2"/>
+      <c r="W111" s="2"/>
+      <c r="X111" s="2"/>
+    </row>
+    <row r="112" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -20602,8 +21506,11 @@
       <c r="U112" s="2">
         <v>-4.48E-2</v>
       </c>
-    </row>
-    <row r="113" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+      <c r="X112" s="2"/>
+    </row>
+    <row r="113" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -20665,8 +21572,11 @@
       <c r="U113" s="2">
         <v>0.19089999999999999</v>
       </c>
-    </row>
-    <row r="114" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V113" s="2"/>
+      <c r="W113" s="2"/>
+      <c r="X113" s="2"/>
+    </row>
+    <row r="114" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -20712,8 +21622,11 @@
         <v>-2.0497000000000001</v>
       </c>
       <c r="U114" s="2"/>
-    </row>
-    <row r="115" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V114" s="2"/>
+      <c r="W114" s="2"/>
+      <c r="X114" s="2"/>
+    </row>
+    <row r="115" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -20759,8 +21672,11 @@
         <v>0.48230000000000001</v>
       </c>
       <c r="U115" s="2"/>
-    </row>
-    <row r="116" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V115" s="2"/>
+      <c r="W115" s="2"/>
+      <c r="X115" s="2"/>
+    </row>
+    <row r="116" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -20806,8 +21722,11 @@
         <v>-0.1956</v>
       </c>
       <c r="U116" s="2"/>
-    </row>
-    <row r="117" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V116" s="2"/>
+      <c r="W116" s="2"/>
+      <c r="X116" s="2"/>
+    </row>
+    <row r="117" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -20839,8 +21758,11 @@
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
-    </row>
-    <row r="118" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V117" s="2"/>
+      <c r="W117" s="2"/>
+      <c r="X117" s="2"/>
+    </row>
+    <row r="118" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -20882,8 +21804,11 @@
         <v>0.4536</v>
       </c>
       <c r="U118" s="2"/>
-    </row>
-    <row r="119" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V118" s="2"/>
+      <c r="W118" s="2"/>
+      <c r="X118" s="2"/>
+    </row>
+    <row r="119" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -20929,8 +21854,11 @@
       <c r="U119" s="2">
         <v>0.2084</v>
       </c>
-    </row>
-    <row r="120" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V119" s="2"/>
+      <c r="W119" s="2"/>
+      <c r="X119" s="2"/>
+    </row>
+    <row r="120" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -20962,8 +21890,11 @@
       <c r="S120" s="2"/>
       <c r="T120" s="2"/>
       <c r="U120" s="2"/>
-    </row>
-    <row r="121" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V120" s="2"/>
+      <c r="W120" s="2"/>
+      <c r="X120" s="2"/>
+    </row>
+    <row r="121" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -20993,8 +21924,11 @@
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
       <c r="U121" s="2"/>
-    </row>
-    <row r="122" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V121" s="2"/>
+      <c r="W121" s="2"/>
+      <c r="X121" s="2"/>
+    </row>
+    <row r="122" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -21024,8 +21958,11 @@
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
-    </row>
-    <row r="123" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V122" s="2"/>
+      <c r="W122" s="2"/>
+      <c r="X122" s="2"/>
+    </row>
+    <row r="123" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -21055,8 +21992,11 @@
       <c r="S123" s="2"/>
       <c r="T123" s="2"/>
       <c r="U123" s="2"/>
-    </row>
-    <row r="124" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V123" s="2"/>
+      <c r="W123" s="2"/>
+      <c r="X123" s="2"/>
+    </row>
+    <row r="124" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -21098,8 +22038,11 @@
         <v>1.0354000000000001</v>
       </c>
       <c r="U124" s="2"/>
-    </row>
-    <row r="125" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V124" s="2"/>
+      <c r="W124" s="2"/>
+      <c r="X124" s="2"/>
+    </row>
+    <row r="125" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -21161,8 +22104,11 @@
       <c r="U125" s="2">
         <v>-0.1988</v>
       </c>
-    </row>
-    <row r="126" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V125" s="2"/>
+      <c r="W125" s="2"/>
+      <c r="X125" s="2"/>
+    </row>
+    <row r="126" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -21192,8 +22138,11 @@
       <c r="S126" s="2"/>
       <c r="T126" s="2"/>
       <c r="U126" s="2"/>
-    </row>
-    <row r="127" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V126" s="2"/>
+      <c r="W126" s="2"/>
+      <c r="X126" s="2"/>
+    </row>
+    <row r="127" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -21251,8 +22200,11 @@
       <c r="U127" s="2">
         <v>0.59189999999999998</v>
       </c>
-    </row>
-    <row r="128" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V127" s="2"/>
+      <c r="W127" s="2"/>
+      <c r="X127" s="2"/>
+    </row>
+    <row r="128" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -21282,8 +22234,11 @@
       <c r="S128" s="2"/>
       <c r="T128" s="2"/>
       <c r="U128" s="2"/>
-    </row>
-    <row r="129" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V128" s="2"/>
+      <c r="W128" s="2"/>
+      <c r="X128" s="2"/>
+    </row>
+    <row r="129" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -21339,8 +22294,11 @@
       <c r="U129" s="2">
         <v>-8.4099999999999994E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V129" s="2"/>
+      <c r="W129" s="2"/>
+      <c r="X129" s="2"/>
+    </row>
+    <row r="130" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -21382,8 +22340,11 @@
         <v>-0.63919999999999999</v>
       </c>
       <c r="U130" s="2"/>
-    </row>
-    <row r="131" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V130" s="2"/>
+      <c r="W130" s="2"/>
+      <c r="X130" s="2"/>
+    </row>
+    <row r="131" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -21427,6 +22388,9 @@
         <v>1.2373000000000001</v>
       </c>
       <c r="U131" s="2"/>
+      <c r="V131" s="2"/>
+      <c r="W131" s="2"/>
+      <c r="X131" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21441,6 +22405,7 @@
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J8" sqref="J8:J9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24716,11 +25681,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9731FF-03B2-4426-AE23-D30863E9EDE7}">
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N23:N24"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24771,7 +25737,7 @@
         <v>489</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>0</v>
@@ -26036,12 +27002,8 @@
         <v>524</v>
       </c>
       <c r="E62" s="19"/>
-      <c r="F62" s="15">
-        <v>139</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>139</v>
-      </c>
+      <c r="F62" s="15"/>
+      <c r="G62" s="18"/>
       <c r="H62" s="17"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -26095,10 +27057,10 @@
       </c>
       <c r="E65" s="16"/>
       <c r="F65" s="15">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>125</v>
+        <v>672</v>
       </c>
       <c r="H65" s="17"/>
     </row>
@@ -26109,10 +27071,10 @@
       <c r="D66" s="15"/>
       <c r="E66" s="16"/>
       <c r="F66" s="15">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>527</v>
+        <v>125</v>
       </c>
       <c r="H66" s="17"/>
     </row>
@@ -26121,7 +27083,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C67" s="15">
         <v>33</v>
@@ -26131,10 +27093,10 @@
       </c>
       <c r="E67" s="16"/>
       <c r="F67" s="15">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>126</v>
+        <v>671</v>
       </c>
       <c r="H67" s="17"/>
     </row>
@@ -26145,10 +27107,10 @@
       <c r="D68" s="15"/>
       <c r="E68" s="16"/>
       <c r="F68" s="15">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>529</v>
+        <v>126</v>
       </c>
       <c r="H68" s="17"/>
     </row>
@@ -26237,20 +27199,20 @@
         <v>69</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>534</v>
+        <v>674</v>
       </c>
       <c r="C73" s="15">
         <v>37</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="15">
         <v>130</v>
       </c>
       <c r="G73" s="18" t="s">
-        <v>130</v>
+        <v>673</v>
       </c>
       <c r="H73" s="21"/>
     </row>
@@ -26281,13 +27243,13 @@
         <v>71</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C75" s="15">
         <v>38</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E75" s="16"/>
       <c r="F75" s="15">
@@ -26303,13 +27265,13 @@
         <v>72</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C76" s="15">
         <v>39</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E76" s="16"/>
       <c r="F76" s="15"/>
@@ -26327,7 +27289,7 @@
         <v>39</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E77" s="16"/>
       <c r="F77" s="15">
@@ -26409,20 +27371,20 @@
         <v>77</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C81" s="15">
         <v>41</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E81" s="16"/>
       <c r="F81" s="15">
         <v>48</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H81" s="17"/>
     </row>
@@ -26431,13 +27393,13 @@
         <v>78</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C82" s="15">
         <v>42</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E82" s="19"/>
       <c r="F82" s="15">
@@ -26453,13 +27415,13 @@
         <v>79</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C83" s="15">
         <v>42</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E83" s="19"/>
       <c r="F83" s="15">
@@ -26475,13 +27437,13 @@
         <v>80</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C84" s="15">
         <v>42</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E84" s="19"/>
       <c r="F84" s="15">
@@ -26497,7 +27459,7 @@
         <v>81</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C85" s="15">
         <v>5</v>
@@ -26519,7 +27481,7 @@
         <v>82</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C86" s="15">
         <v>5</v>
@@ -26559,7 +27521,7 @@
         <v>84</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C88" s="15">
         <v>43</v>
@@ -26599,13 +27561,13 @@
         <v>86</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C90" s="15">
         <v>46</v>
       </c>
       <c r="D90" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E90" s="24"/>
       <c r="F90" s="15"/>
@@ -26617,13 +27579,13 @@
         <v>87</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C91" s="15">
         <v>46</v>
       </c>
       <c r="D91" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E91" s="24"/>
       <c r="F91" s="15"/>
@@ -26635,13 +27597,13 @@
         <v>88</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C92" s="15">
         <v>46</v>
       </c>
       <c r="D92" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E92" s="24"/>
       <c r="F92" s="15"/>
@@ -26653,13 +27615,13 @@
         <v>89</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C93" s="15">
         <v>46</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E93" s="24"/>
       <c r="F93" s="15"/>
@@ -26677,7 +27639,7 @@
         <v>47</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E94" s="16"/>
       <c r="F94" s="15">
@@ -26699,7 +27661,7 @@
         <v>47</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E95" s="16"/>
       <c r="F95" s="15">
@@ -26715,13 +27677,13 @@
         <v>93</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C96" s="15">
         <v>49</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E96" s="16"/>
       <c r="F96" s="15"/>
@@ -26739,7 +27701,7 @@
         <v>49</v>
       </c>
       <c r="D97" s="15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E97" s="16"/>
       <c r="F97" s="15">
@@ -26761,7 +27723,7 @@
         <v>47</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="15">
@@ -26777,13 +27739,13 @@
         <v>101</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C99" s="22">
         <v>48</v>
       </c>
       <c r="D99" s="22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E99" s="16"/>
       <c r="F99" s="22">
@@ -26799,13 +27761,13 @@
         <v>102</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C100" s="22">
         <v>48</v>
       </c>
       <c r="D100" s="22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="22">
@@ -26821,13 +27783,13 @@
         <v>103</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C101" s="22">
         <v>48</v>
       </c>
       <c r="D101" s="22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="22">
@@ -26843,13 +27805,13 @@
         <v>104</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C102" s="26">
         <v>52</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F102" s="22"/>
       <c r="G102" s="23"/>
@@ -26860,13 +27822,13 @@
         <v>105</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C103" s="26">
         <v>52</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F103" s="22"/>
       <c r="G103" s="23"/>
@@ -26877,13 +27839,13 @@
         <v>106</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C104" s="26">
         <v>52</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="23"/>
@@ -26894,13 +27856,13 @@
         <v>107</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C105" s="26">
         <v>53</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="23"/>
@@ -26911,13 +27873,13 @@
         <v>108</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C106" s="26">
         <v>53</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F106" s="22"/>
       <c r="G106" s="23"/>
@@ -26928,13 +27890,13 @@
         <v>109</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C107" s="26">
         <v>53</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="23"/>
@@ -26945,13 +27907,13 @@
         <v>110</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C108" s="26">
         <v>56</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F108" s="22">
         <v>117</v>
@@ -26966,13 +27928,13 @@
         <v>111</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C109" s="26">
         <v>56</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F109" s="22">
         <v>143</v>
@@ -26987,13 +27949,13 @@
         <v>112</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C110" s="26">
         <v>55</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F110" s="22">
         <v>144</v>
@@ -27008,13 +27970,13 @@
         <v>113</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C111" s="26">
         <v>55</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F111" s="22">
         <v>79</v>
@@ -27029,13 +27991,13 @@
         <v>114</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C112" s="26">
         <v>55</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F112" s="22">
         <v>69</v>
@@ -27050,13 +28012,13 @@
         <v>119</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C113" s="26">
         <v>53</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F113" s="22">
         <v>70</v>
@@ -27134,13 +28096,13 @@
         <v>153</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C117" s="26">
         <v>53</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F117" s="15">
         <v>17</v>
@@ -27155,13 +28117,13 @@
         <v>178</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C118" s="26">
         <v>84</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F118" s="15">
         <v>18</v>
@@ -27176,13 +28138,13 @@
         <v>179</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C119" s="26">
         <v>85</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F119" s="22">
         <v>32</v>
@@ -27197,13 +28159,13 @@
         <v>184</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C120" s="26">
         <v>84</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F120" s="22">
         <v>35</v>
@@ -27218,13 +28180,13 @@
         <v>189</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C121" s="26">
         <v>87</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F121" s="22">
         <v>36</v>
@@ -27239,13 +28201,13 @@
         <v>195</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C122" s="26">
         <v>89</v>
       </c>
       <c r="D122" s="26" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F122" s="22">
         <v>37</v>
@@ -27260,13 +28222,13 @@
         <v>196</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C123" s="26">
         <v>90</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F123" s="22">
         <v>39</v>
@@ -27281,13 +28243,13 @@
         <v>197</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C124" s="26">
         <v>91</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F124" s="15">
         <v>42</v>
@@ -27302,13 +28264,13 @@
         <v>201</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C125" s="26">
         <v>93</v>
       </c>
       <c r="D125" s="26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F125" s="15">
         <v>43</v>
@@ -27323,13 +28285,13 @@
         <v>209</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C126" s="26">
         <v>98</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F126" s="15">
         <v>45</v>
@@ -27344,13 +28306,13 @@
         <v>210</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C127" s="26">
         <v>98</v>
       </c>
       <c r="D127" s="26" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F127" s="22">
         <v>46</v>
@@ -27365,13 +28327,13 @@
         <v>211</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C128" s="26">
         <v>99</v>
       </c>
       <c r="D128" s="26" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F128" s="22">
         <v>47</v>
@@ -27386,13 +28348,13 @@
         <v>220</v>
       </c>
       <c r="B129" s="29" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C129" s="29">
         <v>90</v>
       </c>
       <c r="D129" s="29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F129" s="22">
         <v>52</v>
@@ -27799,71 +28761,71 @@
       <c r="H173" s="21"/>
     </row>
     <row r="174" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F174" s="22">
-        <v>140</v>
-      </c>
-      <c r="G174" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H174" s="21"/>
+      <c r="F174" s="15">
+        <v>139</v>
+      </c>
+      <c r="G174" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H174" s="17"/>
     </row>
     <row r="175" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F175" s="22">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G175" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H175" s="21"/>
     </row>
     <row r="176" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F176" s="22">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G176" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H176" s="21"/>
     </row>
     <row r="177" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F177" s="22">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G177" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H177" s="21"/>
     </row>
     <row r="178" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F178" s="22">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G178" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H178" s="21"/>
     </row>
     <row r="179" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F179" s="22">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G179" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H179" s="21"/>
     </row>
     <row r="180" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F180" s="22">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G180" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H180" s="21"/>
     </row>
     <row r="181" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F181" s="22">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G181" s="23" t="s">
         <v>148</v>
@@ -27872,678 +28834,687 @@
     </row>
     <row r="182" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F182" s="22">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G182" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H182" s="21"/>
     </row>
     <row r="183" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F183" s="22">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G183" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H183" s="21"/>
     </row>
     <row r="184" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F184" s="22">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G184" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H184" s="21"/>
     </row>
     <row r="185" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F185" s="22">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G185" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H185" s="21"/>
     </row>
     <row r="186" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F186" s="22">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G186" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H186" s="21"/>
     </row>
     <row r="187" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F187" s="22">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G187" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H187" s="21"/>
     </row>
     <row r="188" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F188" s="22">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G188" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H188" s="21"/>
     </row>
     <row r="189" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F189" s="22">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G189" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H189" s="21"/>
     </row>
     <row r="190" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F190" s="22">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G190" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H190" s="21"/>
     </row>
     <row r="191" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F191" s="22">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G191" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H191" s="21"/>
     </row>
     <row r="192" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F192" s="22">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G192" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H192" s="21"/>
     </row>
     <row r="193" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F193" s="22">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G193" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H193" s="21"/>
     </row>
     <row r="194" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F194" s="22">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G194" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H194" s="21"/>
     </row>
     <row r="195" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F195" s="22">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G195" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H195" s="21"/>
     </row>
     <row r="196" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F196" s="22">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G196" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H196" s="21"/>
     </row>
     <row r="197" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F197" s="22">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G197" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H197" s="21"/>
     </row>
     <row r="198" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F198" s="22">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G198" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H198" s="21"/>
     </row>
     <row r="199" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F199" s="22">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G199" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H199" s="21"/>
     </row>
     <row r="200" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F200" s="22">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G200" s="23" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H200" s="21"/>
     </row>
     <row r="201" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F201" s="22">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G201" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H201" s="21"/>
     </row>
     <row r="202" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F202" s="22">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G202" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H202" s="21"/>
     </row>
     <row r="203" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F203" s="22">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G203" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H203" s="21"/>
     </row>
     <row r="204" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F204" s="22">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G204" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H204" s="21"/>
     </row>
     <row r="205" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F205" s="22">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G205" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H205" s="21"/>
     </row>
     <row r="206" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F206" s="22">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G206" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H206" s="21"/>
     </row>
     <row r="207" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F207" s="22">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G207" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H207" s="21"/>
     </row>
     <row r="208" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F208" s="22">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G208" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H208" s="21"/>
     </row>
     <row r="209" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F209" s="22">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G209" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H209" s="21"/>
     </row>
     <row r="210" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F210" s="22">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G210" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H210" s="21"/>
     </row>
     <row r="211" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F211" s="22">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G211" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H211" s="21"/>
     </row>
     <row r="212" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F212" s="22">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G212" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H212" s="21"/>
     </row>
     <row r="213" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F213" s="22">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G213" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H213" s="21"/>
     </row>
     <row r="214" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F214" s="22">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G214" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H214" s="21"/>
     </row>
     <row r="215" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F215" s="22">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G215" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H215" s="21"/>
     </row>
     <row r="216" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F216" s="22">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G216" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H216" s="21"/>
     </row>
     <row r="217" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F217" s="22">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G217" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H217" s="21"/>
     </row>
     <row r="218" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F218" s="22">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G218" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H218" s="21"/>
     </row>
     <row r="219" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F219" s="22">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G219" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H219" s="21"/>
     </row>
     <row r="220" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F220" s="22">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G220" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H220" s="21"/>
     </row>
     <row r="221" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F221" s="22">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G221" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H221" s="21"/>
     </row>
     <row r="222" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F222" s="22">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G222" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H222" s="21"/>
     </row>
     <row r="223" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F223" s="22">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G223" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H223" s="21"/>
     </row>
     <row r="224" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F224" s="22">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G224" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H224" s="21"/>
     </row>
     <row r="225" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F225" s="22">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G225" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H225" s="21"/>
     </row>
     <row r="226" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F226" s="22">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G226" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H226" s="21"/>
     </row>
     <row r="227" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F227" s="22">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G227" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H227" s="21"/>
     </row>
     <row r="228" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F228" s="22">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G228" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H228" s="21"/>
     </row>
     <row r="229" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F229" s="22">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G229" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H229" s="21"/>
     </row>
     <row r="230" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F230" s="22">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G230" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H230" s="21"/>
     </row>
     <row r="231" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F231" s="22">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G231" s="23" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="H231" s="21"/>
     </row>
     <row r="232" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F232" s="22">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G232" s="23" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="H232" s="21"/>
     </row>
     <row r="233" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F233" s="22">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G233" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H233" s="21"/>
     </row>
     <row r="234" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F234" s="22">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G234" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H234" s="21"/>
     </row>
     <row r="235" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F235" s="22">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G235" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H235" s="21"/>
     </row>
     <row r="236" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F236" s="22">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G236" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H236" s="21"/>
     </row>
     <row r="237" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F237" s="22">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G237" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H237" s="21"/>
     </row>
     <row r="238" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F238" s="22">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G238" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H238" s="21"/>
     </row>
     <row r="239" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F239" s="22">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G239" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H239" s="21"/>
     </row>
     <row r="240" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F240" s="22">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G240" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H240" s="21"/>
     </row>
     <row r="241" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F241" s="22">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G241" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H241" s="21"/>
     </row>
     <row r="242" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F242" s="22">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G242" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H242" s="21"/>
     </row>
     <row r="243" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F243" s="22">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G243" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H243" s="21"/>
     </row>
     <row r="244" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F244" s="22">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G244" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H244" s="21"/>
     </row>
     <row r="245" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F245" s="22">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G245" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H245" s="21"/>
     </row>
     <row r="246" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F246" s="22">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G246" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H246" s="21"/>
     </row>
     <row r="247" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F247" s="22">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G247" s="23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H247" s="21"/>
     </row>
     <row r="248" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F248" s="22">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G248" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H248" s="21"/>
     </row>
     <row r="249" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F249" s="22">
-        <v>220</v>
-      </c>
-      <c r="G249" s="30" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="G249" s="23" t="s">
+        <v>217</v>
       </c>
       <c r="H249" s="21"/>
     </row>
     <row r="250" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F250" s="22">
-        <v>23</v>
-      </c>
-      <c r="G250" s="23" t="s">
-        <v>23</v>
+        <v>220</v>
+      </c>
+      <c r="G250" s="30" t="s">
+        <v>218</v>
       </c>
       <c r="H250" s="21"/>
     </row>
     <row r="251" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F251" s="22">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G251" s="23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H251" s="21"/>
     </row>
     <row r="252" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F252" s="22">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G252" s="23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H252" s="21"/>
     </row>
     <row r="253" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F253" s="22">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G253" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H253" s="21"/>
     </row>
     <row r="254" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F254" s="22">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G254" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H254" s="21"/>
     </row>
     <row r="255" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F255" s="22">
+        <v>26</v>
+      </c>
+      <c r="G255" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H255" s="21"/>
+    </row>
+    <row r="256" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F256" s="22">
         <v>27</v>
       </c>
-      <c r="G255" s="23" t="s">
+      <c r="G256" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H255" s="21"/>
-    </row>
-    <row r="256" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F256" s="32">
+      <c r="H256" s="21"/>
+    </row>
+    <row r="257" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F257" s="32">
         <v>28</v>
       </c>
-      <c r="G256" s="33" t="s">
+      <c r="G257" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="H256" s="31"/>
+      <c r="H257" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CDK integration + SMILES PARSING
</commit_message>
<xml_diff>
--- a/data/HukkerikarEnvironmental.xlsx
+++ b/data/HukkerikarEnvironmental.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115" tabRatio="724" activeTab="1" xr2:uid="{B1B8E9E2-0821-49EE-A8A7-D989EA31A508}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8790" activeTab="1" xr2:uid="{9DF4B5E0-0503-411D-9815-9AD522F5F236}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8790" activeTab="3" xr2:uid="{9DF4B5E0-0503-411D-9815-9AD522F5F236}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstOrder" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="ThirdOrder" sheetId="4" r:id="rId3"/>
     <sheet name="Unifac-Equivalences" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027" refMode="R1C1"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3146,7 +3145,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2705E1D5-5341-4401-BFD2-EC8497DDB141}" name="Table2" displayName="Table2" ref="A1:D129" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2705E1D5-5341-4401-BFD2-EC8497DDB141}" name="Table2" displayName="Table2" ref="A1:D130" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{97ACAD8E-9361-4D28-8EB8-A9AAF9F8DCA2}" name="Column1" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{26DFE1A7-791C-482C-BA42-0807897D8853}" name="UNIFAC" dataDxfId="10"/>
@@ -3467,10 +3466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CF915C-548F-44E5-A457-8BD61E3FF56A}">
   <dimension ref="A1:X221"/>
   <sheetViews>
-    <sheetView topLeftCell="I74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L190" sqref="L190"/>
-    </sheetView>
-    <sheetView topLeftCell="A22" workbookViewId="1">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -15423,10 +15419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F60655-82C2-4DD7-8FC9-7DBEF022EFA3}">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22402,10 +22395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760C7225-5CC2-473E-91AB-7F8F99835134}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25683,10 +25673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9731FF-03B2-4426-AE23-D30863E9EDE7}">
   <dimension ref="A1:H257"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26980,12 +26969,8 @@
         <v>524</v>
       </c>
       <c r="E61" s="19"/>
-      <c r="F61" s="15">
-        <v>138</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>138</v>
-      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="18"/>
       <c r="H61" s="17"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -27002,8 +26987,12 @@
         <v>524</v>
       </c>
       <c r="E62" s="19"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="18"/>
+      <c r="F62" s="15">
+        <v>138</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>138</v>
+      </c>
       <c r="H62" s="17"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -27801,28 +27790,20 @@
       <c r="H101" s="21"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="26">
-        <v>104</v>
-      </c>
-      <c r="B102" s="26" t="s">
-        <v>556</v>
-      </c>
-      <c r="C102" s="26">
-        <v>52</v>
-      </c>
-      <c r="D102" s="26" t="s">
-        <v>557</v>
-      </c>
+      <c r="A102" s="21"/>
+      <c r="B102" s="22"/>
+      <c r="C102" s="22"/>
+      <c r="D102" s="22"/>
       <c r="F102" s="22"/>
       <c r="G102" s="23"/>
       <c r="H102" s="21"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="26">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C103" s="26">
         <v>52</v>
@@ -27836,10 +27817,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="26">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C104" s="26">
         <v>52</v>
@@ -27853,16 +27834,16 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="26">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C105" s="26">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="23"/>
@@ -27870,10 +27851,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="26">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C106" s="26">
         <v>53</v>
@@ -27887,10 +27868,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="26">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C107" s="26">
         <v>53</v>
@@ -27903,17 +27884,17 @@
       <c r="H107" s="21"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="27">
-        <v>110</v>
+      <c r="A108" s="26">
+        <v>109</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C108" s="26">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F108" s="22">
         <v>117</v>
@@ -27925,10 +27906,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="27">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C109" s="26">
         <v>56</v>
@@ -27946,16 +27927,16 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="27">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C110" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F110" s="22">
         <v>144</v>
@@ -27967,10 +27948,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="27">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C111" s="26">
         <v>55</v>
@@ -27988,10 +27969,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="27">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C112" s="26">
         <v>55</v>
@@ -28009,16 +27990,16 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="27">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C113" s="26">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="F113" s="22">
         <v>70</v>
@@ -28030,16 +28011,16 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="27">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>143</v>
+        <v>571</v>
       </c>
       <c r="C114" s="26">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>144</v>
+        <v>561</v>
       </c>
       <c r="F114" s="22">
         <v>10</v>
@@ -28051,10 +28032,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="27">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C115" s="26">
         <v>61</v>
@@ -28072,10 +28053,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="27">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C116" s="26">
         <v>61</v>
@@ -28093,16 +28074,16 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="27">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>572</v>
+        <v>145</v>
       </c>
       <c r="C117" s="26">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>561</v>
+        <v>144</v>
       </c>
       <c r="F117" s="15">
         <v>17</v>
@@ -28114,16 +28095,16 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="27">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C118" s="26">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="F118" s="15">
         <v>18</v>
@@ -28135,16 +28116,16 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="27">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C119" s="26">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F119" s="22">
         <v>32</v>
@@ -28156,16 +28137,16 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="27">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C120" s="26">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="F120" s="22">
         <v>35</v>
@@ -28177,16 +28158,16 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="27">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C121" s="26">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="F121" s="22">
         <v>36</v>
@@ -28198,16 +28179,16 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="27">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C122" s="26">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D122" s="26" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F122" s="22">
         <v>37</v>
@@ -28219,16 +28200,16 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="27">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C123" s="26">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F123" s="22">
         <v>39</v>
@@ -28240,16 +28221,16 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="27">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C124" s="26">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F124" s="15">
         <v>42</v>
@@ -28261,16 +28242,16 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="27">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C125" s="26">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D125" s="26" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F125" s="15">
         <v>43</v>
@@ -28282,16 +28263,16 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="27">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C126" s="26">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F126" s="15">
         <v>45</v>
@@ -28303,10 +28284,10 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="27">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C127" s="26">
         <v>98</v>
@@ -28324,16 +28305,16 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="27">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C128" s="26">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D128" s="26" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F128" s="22">
         <v>47</v>
@@ -28344,17 +28325,17 @@
       <c r="H128" s="21"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="28">
-        <v>220</v>
-      </c>
-      <c r="B129" s="29" t="s">
-        <v>590</v>
-      </c>
-      <c r="C129" s="29">
-        <v>90</v>
-      </c>
-      <c r="D129" s="29" t="s">
-        <v>583</v>
+      <c r="A129" s="27">
+        <v>211</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>589</v>
+      </c>
+      <c r="C129" s="26">
+        <v>99</v>
+      </c>
+      <c r="D129" s="26" t="s">
+        <v>589</v>
       </c>
       <c r="F129" s="22">
         <v>52</v>
@@ -28365,6 +28346,18 @@
       <c r="H129" s="21"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="28">
+        <v>220</v>
+      </c>
+      <c r="B130" s="29" t="s">
+        <v>590</v>
+      </c>
+      <c r="C130" s="29">
+        <v>90</v>
+      </c>
+      <c r="D130" s="29" t="s">
+        <v>583</v>
+      </c>
       <c r="F130" s="22">
         <v>53</v>
       </c>

</xml_diff>